<commit_message>
Fixed rebound on home position from forward move
</commit_message>
<xml_diff>
--- a/les_petits_chevaux/test/board_test.xlsx
+++ b/les_petits_chevaux/test/board_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="3">
   <si>
     <t>H</t>
   </si>
@@ -480,12 +480,12 @@
   <dimension ref="L4:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AI13" sqref="AI13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="2.21875" style="1"/>
+    <col min="1" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="12:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -567,8 +567,8 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="1" t="s">
-        <v>1</v>
+      <c r="R8" s="1">
+        <v>11</v>
       </c>
       <c r="S8" s="1">
         <v>3</v>

</xml_diff>